<commit_message>
Ahora sí, último commit sin los prints de los links
Co-Authored-By: claribernhardt <177650472+claribernhardt@users.noreply.github.com>
Co-Authored-By: roluque <177880187+roluque@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/TP1/links-Bernhadt_Laszeski_Luque.xlsx
+++ b/TP1/links-Bernhadt_Laszeski_Luque.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A129"/>
+  <dimension ref="A1:A116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,894 +443,803 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/nuevo-round-cristina-kirchner-le-dijo-a-milei-que-hace-plagio-y-que-se-dedica-a-boludear-en-redes-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//politica/detuvieron-a-un-hombre-de-40-anos-por-el-paquete-explosivo-contra-la-sociedad-rural-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/uno-de-los-auditorias-mas-selectos-del-pais-espera-la-respuesta-de-milei-a-cristina-kirchner-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//politica/javier-milei-y-robespierre-a-los-decretazos-para-la-revolucion-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/la-casa-rosada-reforzo-controles-tras-el-ataque-a-la-sociedad-rural-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//deportes/futbol/marca-una-era-lionel-scaloni-cumple-6-anos-dirigiendo-a-la-seleccion-argentina-y-lo-celebra-con-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/un-frente-gremial-desorientado-expuesto-y-dividido-es-la-pesadilla-de-los-pasajeros-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//politica/bullrich-hablo-sobre-el-video-de-firmenich-y-se-desmarco-de-villarruel-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//sociedad/alerta-en-cordoba-controlaron-el-incendio-camino-a-carlos-paz-pero-hay-otros-dos-focos-activos-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//el-mundo/venezuela-busca-quitar-a-brasil-la-custodia-de-la-embajada-argentina-en-caracas-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//seguridad/por-una-mula-nerviosa-que-estaba-por-viajar-a-paris-descubrieron-una-banda-que-traficaba-cocaina-a-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//sociedad/avalancha-en-bariloche-la-operadora-del-911-relato-como-mantuvo-despierto-al-joven-atrapado-en-la-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/el-gobierno-le-pidio-a-la-corte-penal-internacional-la-detencion-de-maduro-y-otros-cabecillas-del-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//el-mundo/gira-papal-papua-nueva-guinea-el-pais-que-tenia-todo-para-ser-un-paraiso-y-hoy-es-una-de-las-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/ramon-diaz-el-refugio-rural-desde-donde-una-de-las-glorias-de-river-planea-otra-vida-y-habla-sin-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//comunidad/hambre-de-futuro/como-viven-los-chicos-donde-la-falta-de-atencion-medica-y-pediatrica-los-lleva-a-la-muerte-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/economia-buscara-impedir-que-los-intendentes-incluyan-tasas-municipales-en-las-boletas-de-servicios-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//politica/el-negocio-de-ser-senador-un-sueldo-de-casi-8000000-y-una-caja-minima-para-contratar-personal-de-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/futbol/nations-league-italia-sufrio-un-gol-insolito-a-los-13-segundos-pero-se-recupero-y-le-gano-a-francia-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//politica/de-economia-no-entendes-mucho-la-secuencia-de-golpes-y-contragolpes-en-x-entre-javier-milei-y-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/el-presidente-del-bcra-santiago-bausili-sobre-el-fmi-un-socio-que-no-pone-dinero-es-mas-bien-un-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//politica/dura-respuesta-de-pablo-moyano-a-la-carta-de-cristina-kirchner-con-criticas-al-peronismo-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//seguridad/por-una-mula-nerviosa-que-estaba-por-viajar-a-paris-descubrieron-una-banda-que-traficaba-cocaina-a-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//opinion/javi-kari-y-caputin-si-es-lo-que-hay-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/dolar/disputa-entre-milei-y-cristina-kirchner-hernan-lacunza-intervino-en-la-discusion-y-dijo-que-en-algo-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//opinion/la-logica-del-reality-invadio-a-la-politica-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/futbol/nations-league-italia-sufrio-un-gol-insolito-a-los-13-segundos-pero-se-recupero-y-le-gano-a-francia-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//politica/elecciones-estudiantiles-se-afianzan-en-la-uba-el-liderazgo-del-frente-reformista-y-el-perfil-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//revista-lugares/cordoba-la-historia-del-colegio-mas-antiguo-del-pais-que-aun-conserva-cofradias-y-ensena-latin-y-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//seguridad/la-ministra-patricia-bullrich-creo-un-comando-unificado-para-proteger-la-actividad-comercial-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/no-nos-van-a-callar-el-presidente-de-la-rural-califico-al-atentado-de-un-episodio-de-una-argentina-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//seguridad/el-tunel-en-san-isidro-la-enigmatica-desaparicion-de-una-camioneta-y-las-misteriosas-comidas-que-le-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//sociedad/las-cifras-del-paro-la-medida-afecto-a-16000-pasajeros-de-185-vuelos-en-aeroparque-y-ezeiza-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//sociedad/adios-a-melina-furman-la-pensadora-de-la-educacion-mas-influyente-en-habla-hispana-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/reves-para-alberto-fernandez-casacion-rechazo-apartar-al-juez-ercolini-de-la-causa-de-los-seguros-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//sociedad/consejos-de-expertos-guardar-pastillas-en-la-cocina-o-el-bano-y-otros-errores-comunes-que-se-cometen-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//sociedad/avalancha-en-bariloche-la-justicia-investiga-el-rol-de-los-sobrevivientes-en-la-tragedia-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//economia/negocios/el-local-argentino-que-impuso-las-medialunas-en-una-capital-gastronomica-mundial-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/personajes/monica-cahen-danvers-como-vive-hoy-una-de-las-figuras-mas-queridas-de-la-television-a-casi-dos-anos-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//el-mundo/el-supertifon-yagi-llego-a-vietnam-con-vientos-arrasadores-al-menos-4-muertos-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//propiedades/casas-y-departamentos/alquileres-cuanto-cuesta-un-departamento-por-mes-barrio-por-barrio-en-la-ciudad-de-buenos-aires-nid02042024/</t>
+          <t>https://www.lanacion.com.ar//lifestyle/maxima-en-buenos-aires-la-intimidad-de-la-fiesta-de-cumpleanos-80-de-su-madre-en-el-yatch-club-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/agustin-romo-el-militante-mileista-que-detesta-a-macri-y-que-caputo-eligio-para-liderar-el-bloque-de-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//sociedad/murio-melina-furman-la-ultima-entrevista-de-la-cientifica-con-la-nacion-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/como-sera-el-nuevo-indice-de-inflacion-que-anuncio-el-indec-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//deportes/la-agenda-de-la-tv-del-sabado-boca-vs-talleres-los-pumas-vs-wallabies-la-nations-league-europea-y-la-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//lifestyle/hija-de-una-argentina-la-foto-que-delato-la-relacion-entre-el-principe-felipe-e-isabel-sartorius-el-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//seguridad/por-una-mula-nerviosa-que-estaba-por-viajar-a-paris-descubrieron-una-banda-que-traficaba-cocaina-a-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//sabado/en-francia-100-puntos-para-un-malbec-argentino-en-el-mercado-de-vinos-de-lujo-mas-top-del-mundo-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//estados-unidos/fin-a-otro-drama-de-boeing-la-capsula-starliner-volvio-a-la-tierra-y-dejo-a-dos-astronautas-varados-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//cultura/como-conocer-buenos-aires-a-traves-de-lecturas-y-librerias-que-recomienda-samanta-schweblin-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//propiedades/casas-y-departamentos/historias-es-argentino-compro-un-burdel-para-crear-un-corredor-en-zona-norte-y-hara-un-cable-carril-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/javier-milei-ya-dio-casi-seis-vueltas-al-mundo-desde-que-es-presidente-y-gasto-us24-millones-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//tecnologia/la-sutil-diferencia-entre-soberania-y-censura-previa-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/futbol/la-crisis-en-la-seleccion-de-chile-arturo-vidal-apunto-contra-gareca-y-mauricio-isla-anticipa-una-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//deportes/tenis/juegos-paralimpicos-gustavo-fernandez-consiguio-la-medalla-de-bronce-en-paris-y-lo-festejo-a-pura-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/futbol/la-gran-cantidad-de-partidos-amenaza-la-salud-de-los-futbolistas-datos-revelaciones-y-conclusiones-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//deportes/natacion/jincheng-guo-el-nadador-chino-que-es-como-un-misil-y-asombra-al-mundo-en-los-juegos-paralimpicos-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/rugby/santiago-grondona-se-perdio-el-mundial-por-una-lesion-y-esta-de-vuelta-en-los-pumas-en-una-zona-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//deportes/rugby/los-pumas-australia-por-el-rugby-championship-la-seleccion-argentina-pasa-al-calor-de-santa-fe-con-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//salud/cuanto-sabes-sobre-los-primeros-anos-de-tu-hijo-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//el-mundo/el-popular-pastor-evangelico-que-encabezara-una-marcha-con-bolsonaro-y-pedira-carcel-para-el-juez-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/inflacion-de-marzo-el-ipc-en-la-ciudad-fue-de-132-y-acumulo-573-en-tres-meses-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//ideas/dahlia-scheindlin-la-relacion-entre-israelies-y-palestinos-es-la-peor-jamas-vivida-en-la-region-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/mariano-recalde-definio-la-postura-kirchnerista-sobre-lijo-esta-propuesta-de-milei-para-la-corte-no-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//el-mundo/elecciones-en-eeuu-como-es-la-creciente-influencia-de-elon-musk-sobre-donald-trump-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//cultura/repercusiones-de-un-discurso-anticientifico-contra-los-periodistas-intelectuales-y-artistas-amigos-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//economia/campo/ramon-diaz-el-refugio-rural-desde-donde-una-de-las-glorias-de-river-planea-otra-vida-y-habla-sin-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/nuevo-testigo-el-martes-declarara-otro-medico-que-vio-el-moreton-en-el-ojo-de-fabiola-yanez-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//revista-jardin/una-forma-inteligente-de-sostener-la-arquitectura-esconder-el-estacionamiento-y-lograr-intimidad-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/aerolineas-apunto-a-los-gremios-por-el-paro-revelo-cuanto-ganan-los-pilotos-e-insistio-con-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//espectaculos/yanina-latorre-adelanto-quien-ganaria-el-martin-fierro-de-oro-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/nada-sera-igual-las-24-horas-freneticas-y-de-incertidumbre-que-tras-el-atentado-cambiaron-para-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//sabado/un-clasico-de-la-parrilla-julio-iglesias-mandaba-un-avion-para-hacerse-llevar-los-bifes-a-brasil-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/juan-grabois-compartira-con-francisco-en-roma-un-nuevo-encuentro-con-los-movimientos-populares-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//revista-lugares/la-ruta-de-los-abstemios-planes-entre-las-bodegas-mendocinas-sin-tomar-vino-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/dolar-el-bcra-deberia-comprar-mas-de-us60-millones-por-dia-para-cumplir-la-meta-del-fmi-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//salud/el-mercado-de-los-sabores-exoticos-y-otros-platos-para-paladares-exigentes-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//el-mundo/un-supertifon-azota-el-sur-de-china-con-vientos-de-245-kmh-hay-evacuaciones-masivas-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//espectaculos/personajes/lady-gaga-hizo-una-importante-confesion-vinculada-a-su-salud-no-fumo-marihuana-desde-hace-anos-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//el-mundo/las-nueras-del-hombre-acusado-en-francia-por-las-violaciones-a-su-mujer-revelaron-mas-detalles-del-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//ideas/lecturas-las-grandes-cuentos-de-una-escritora-marcada-por-la-tragedia-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//estados-unidos/alivio-para-donald-trump-retrasan-para-despues-de-las-elecciones-la-sentencia-del-juicio-por-el-pago-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//espectaculos/personajes/valeria-lynch-sus-dias-entre-uruguay-y-la-argentina-el-motivo-por-el-que-no-volveria-a-casarse-y-por-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//el-mundo/analizan-cobrar-el-acceso-a-la-fontana-di-trevi-la-emblematica-fuente-en-roma-donde-se-piden-deseos-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//revista-hola/trabajo-en-patito-feo-santiago-talledo-todo-era-desesperante-un-dia-le-dije-a-mi-mama-no-quiero-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/novedades-en-los-medios-el-observador-1079-presenta-nuevos-programas-ronnie-arias-dejo-pop-y-radio-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//autos/en-que-paises-sirve-la-licencia-de-conducir-argentina-y-cual-es-el-requisito-extra-para-poder-usarla-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//el-mundo/el-caso-contra-bella-nilsson-la-reina-de-la-basura-acusada-del-mayor-crimen-ambiental-en-la-historia-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//economia/campo/un-lujo-lleno-el-tanque-de-la-camioneta-y-se-quedo-atonico-por-lo-que-tuvo-que-pagar-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//autos/cuanto-cuestan-las-pick-ups-en-septiembre-luego-de-la-baja-de-precios-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//juegos/trivias/trivia-exclusiva-cuanto-sabes-sobre-las-mejores-comidas-del-mundo-nid02092024/</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/futbol/el-futbol-y-la-llegada-de-las-sad-de-menem-a-milei-los-proyectos-que-pasaba-con-los-clubes-y-el-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//sabado/solo-vos-podes-salvarte-gabriel-oliveri-y-una-vida-5-estrellas-su-amistad-con-pampita-la-visita-de-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/cine/donde-estan-los-clasicos-en-el-streaming-los-grandes-nombres-que-faltan-y-las-peliculas-que-si-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//espectaculos/personajes/la-serie-de-milei-santiago-oria-explica-como-se-financio-por-que-dice-que-no-es-un-cineasta-del-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//autos/no-existe-la-cedula-azul-como-autorizar-a-alguien-a-que-maneje-un-auto-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//espectaculos/personajes/ian-mckellen-fue-lapidario-en-sus-opiniones-sobre-la-reina-elizabeth-ii-el-rey-carlos-iii-y-el-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//revista-lugares/paxos-idilico-destino-griego-que-se-luce-en-una-exitosa-serie-de-tv-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//espectaculos/que-ver-en-netflix-argentina-el-ranking-de-las-10-mejores-peliculas-para-disfrutar-este-fin-de-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//sociedad/devolverle-su-alma-una-fecha-posible-para-que-concluya-la-desafiante-restauracion-de-un-historico-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//espectaculos/cine/una-pregunta-muchas-posibles-respuestas-para-que-sirve-un-festival-de-cine-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/personajes/rocio-hernandez-la-argentina-que-descubrio-nicolas-repetto-trabajo-con-ganadores-del-oscar-y-estrena-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/https://foodit.lanacion.com.ar/novedades-y-tendencias/marinado-papel-aluminio-y-aceite-los-aliados-para-preparar-los-mejores-vegetales-a-parrilla-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/medida-historica-el-gobierno-aprobo-un-sistema-que-permite-reducir-el-tiempo-de-enfriado-de-la-carne-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//espectaculos/personajes/el-gran-seductor-que-triunfo-en-cine-teatro-y-tv-fracaso-cuando-quiso-cambiar-el-rumbo-y-encontro-a-nid05092024/</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/dolares-ypf-y-pampa-energia-captaron-financiamiento-internacional-millonario-en-el-mercado-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//salud/nutricion/claves-nutricionales-para-prevenir-problemas-de-salud-en-la-tercera-edad-nid05092024/</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/negocios/se-hizo-peluquero-por-azar-y-hoy-es-el-elegido-de-las-celebrities-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//juegos/trivias/trivia-exclusiva-cuanto-sabes-sobre-malasia-nid05092024/</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/television/pnp-150-mil-horas-de-video-cruzadas-personales-humor-incomodo-y-la-formula-magica-que-llevo-a-la-tv-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//sociedad/en-avenida-de-mayo-el-hotel-de-lujo-que-hospedo-a-politicos-y-artistas-extranjeros-y-que-hoy-muestra-nid03092024/</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/indiana-cubero-mostro-por-primera-vez-la-cara-de-su-hermano-cruz-la-reaccion-de-nicole-neumann-nid05092024/</t>
+          <t>https://www.lanacion.com.ar//economia/campo/no-nos-van-a-callar-el-presidente-de-la-rural-califico-al-atentado-de-un-episodio-de-una-argentina-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//salud/vida_sana/que-es-la-amnesia-glutea-y-como-puede-prevenirse-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//economia/campo/nada-sera-igual-las-24-horas-freneticas-y-de-incertidumbre-que-tras-el-atentado-cambiaron-para-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//juegos/trivias/trivia-exclusiva-cuanto-sabes-sobre-la-lista-de-schindler-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//economia/campo/131-islas-malvinas-productores-firmaron-un-duro-documento-contra-europa-a-la-que-acusan-de-degradar-nid05092024/</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/personajes/los-looks-de-los-martin-fierro-los-dos-vestidos-de-mirtha-la-conductora-que-evocara-a-hollywood-y-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//economia/campo/seran-us250-millones-este-ano-la-argentina-exportara-un-500-mas-de-azucar-que-en-2023-nid05092024/</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/griselda-siciliani-rompio-el-silencio-y-conto-la-verdad-sobre-su-supuesta-separacion-de-luciano-nid05092024/</t>
+          <t>https://www.lanacion.com.ar//tecnologia/asi-se-veria-campanita-en-la-vida-real-segun-la-inteligencia-artificial-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/que-ver-en-netflix-argentina-el-ranking-de-las-10-mejores-peliculas-para-disfrutar-este-fin-de-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//tecnologia/estos-son-los-iphone-que-no-seran-compatibles-con-la-ia-de-apple-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/personajes/murio-el-periodista-y-presentador-de-mtv-javier-andrade-a-los-58-anos-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//tecnologia/las-cinco-carreras-que-nadie-elige-para-estudiar-en-la-argentina-segun-la-inteligencia-artificial-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//lifestyle/se-enamoraron-en-italia-en-argentina-un-suceso-oscuro-los-alejo-y-30-anos-despues-llegaron-las-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//ideas/javier-milei-de-la-realidad-virtual-al-resultado-economico-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/https://foodit.lanacion.com.ar/recetas/pastafrola-nid21082024/</t>
+          <t>https://www.lanacion.com.ar//opinion/milei-y-el-dilema-de-la-casta-dialoguista-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/personajes/el-gran-seductor-que-triunfo-en-cine-teatro-y-tv-fracaso-cuando-quiso-cambiar-el-rumbo-y-encontro-a-nid05092024/</t>
+          <t>https://www.lanacion.com.ar//opinion/ascenso-y-caida-de-un-cafe-hipster-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//salud/nutricion/claves-nutricionales-para-prevenir-problemas-de-salud-en-la-tercera-edad-nid05092024/</t>
+          <t>https://www.lanacion.com.ar//editoriales/los-liceos-militares-y-la-excelencia-educativa-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//juegos/trivias/trivia-exclusiva-cuanto-sabes-sobre-malasia-nid05092024/</t>
+          <t>https://www.lanacion.com.ar//editoriales/salud-y-cigarrillos-electronicos-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//sociedad/en-avenida-de-mayo-el-hotel-de-lujo-que-hospedo-a-politicos-y-artistas-extranjeros-y-que-hoy-muestra-nid03092024/</t>
+          <t>https://www.lanacion.com.ar//opinion/sin-mas-empleo-no-se-podran-pagar-las-jubilaciones-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/131-islas-malvinas-productores-firmaron-un-duro-documento-contra-europa-a-la-que-acusan-de-degradar-nid05092024/</t>
+          <t>https://www.lanacion.com.ar//espectaculos/antonela-roccuzzo-y-su-intima-amiga-elena-galera-se-robaron-todas-las-miradas-con-sus-looks-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/seran-us250-millones-este-ano-la-argentina-exportara-un-500-mas-de-azucar-que-en-2023-nid05092024/</t>
+          <t>https://www.lanacion.com.ar//lifestyle/mascotas/murio-zanahoria-el-pez-dorado-mas-grande-del-mundo-y-su-edad-sorprendio-a-mas-de-uno-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/logro-del-conicet-revelaron-detalles-de-un-proceso-que-podria-ser-clave-para-el-futuro-de-los-nid04092024/</t>
+          <t>https://www.lanacion.com.ar//lifestyle/cuidado-cuerpo-belleza/la-semilla-negra-que-utilizaban-nuestros-ancestros-para-mejorar-la-digestion-aliviar-la-hinchazon-y-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/asi-quedo-la-oficina-de-nicolas-pino-despues-de-la-explosion-del-paquete-los-detalles-nid05092024/</t>
+          <t>https://www.lanacion.com.ar//lifestyle/por-que-se-celebra-hoy-el-dia-mundial-del-pelirrojo-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//tecnologia/asi-se-veria-campanita-en-la-vida-real-segun-la-inteligencia-artificial-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//lifestyle/en-las-redes/cinco-nombres-de-cosas-comunes-que-quizas-no-conoces-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//tecnologia/estos-son-los-iphone-que-no-seran-compatibles-con-la-ia-de-apple-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//lifestyle/en-las-redes/el-hilo-viral-que-muestra-la-verdad-detras-de-las-escenas-mas-famosas-de-peliculas-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//tecnologia/las-cinco-carreras-que-nadie-elige-para-estudiar-en-la-argentina-segun-la-inteligencia-artificial-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//lifestyle/en-las-redes/las-imagenes-del-punto-mas-letal-de-la-tierra-capaz-de-matar-a-cualquiera-que-se-encuentra-cerca-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/preocupante-regreso-de-tension-y-violencia-nid05092024/</t>
+          <t>https://www.lanacion.com.ar//politica/milei-versus-cristina-el-presidente-le-respondio-a-la-exvicepresidenta-en-el-congreso-del-iaef-y-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/los-esbirros-del-fmi-no-la-ven-nid05092024/</t>
+          <t>https://www.lanacion.com.ar//economia/dolar-hoy-dolar-blue-hoy-a-cuanto-cotiza-este-sabado-7-de-septiembre-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//opinion/dejemos-de-ser-el-peligro-y-seamos-la-solucion-al-cambio-climatico-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//deportes/futbol/eliminatorias-sudamericanas-en-la-noche-de-la-despedida-de-luis-suarez-uruguay-no-encontro-el-gol-y-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//editoriales/mas-perversiones-en-pandemia-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//economia/negocios/el-local-argentino-que-impuso-las-medialunas-en-una-capital-gastronomica-mundial-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//editoriales/el-abuso-de-las-pantallas-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//espectaculos/personajes/ian-mckellen-fue-lapidario-en-sus-opiniones-sobre-la-reina-elizabeth-ii-el-rey-carlos-iii-y-el-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//opinion/estados-contra-las-plataformas-impunidad-o-libertad-de-expresion-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//propiedades/san-fernando-como-paso-de-ser-una-localidad-poco-buscada-de-zona-norte-a-atraer-grandes-inversiones-nid31082024/</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/musica/a-10-anos-de-su-muerte-habra-dos-shows-el-fin-de-semana-para-recordar-a-gustavo-cerati-donde-cuando-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//deportes/boxeo/fernando-pumita-martinez-y-un-dilema-si-va-por-la-revancha-con-ioka-se-expone-a-la-perdida-de-uno-de-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/el-mal-momento-que-atraviesa-brenda-asnicar-tras-la-muerte-de-su-mascota-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//economia/negocios/trei-brundrett-todo-proyecto-de-medios-reflexiona-sobre-la-cultura-las-personas-y-los-resultados-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/asi-se-veia-shakira-en-el-oasis-la-telenovela-colombiana-de-1994-que-quedo-en-el-olvido-por-su-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//economia/negocios/ensenanzas-olimpicas-los-ejecutivos-argentinos-ganan-la-medalla-de-lata-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//lifestyle/cuidado-cuerpo-belleza/el-ejercicio-mental-que-puede-ser-la-clave-para-mantener-el-cerebro-agil-durante-el-envejecimiento-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//economia/negocios/aceptar-la-nueva-version-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//lifestyle/en-las-redes/eclipse-lunar-en-septiembre-de-2024-cuando-sera-donde-y-todas-las-fases-del-fenomeno-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//economia/negocios/calidad-de-trabajo-el-derecho-a-la-desconexion-digital-se-extiende-por-el-mundo-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//estados-unidos/florida/el-hijo-de-monica-de-alzaga-se-volvio-viral-por-su-increible-reaccion-al-presenciar-un-tiroteo-en-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//espectaculos/television/rituales-maquillaje-y-zozobra-como-se-vive-un-partido-de-la-seleccion-desde-una-cabina-de-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//lifestyle/mascotas/alerta-en-madrid-aparecio-un-buitre-leonado-una-de-las-aves-mas-peligrosas-del-mundo-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//espectaculos/personajes/delincuencia-sexual-y-pornografia-infantil-los-oscuros-motivos-por-los-que-jeoffrey-jones-quedo-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//el-mundo/un-supertifon-azota-el-sur-de-china-con-vientos-de-245-kmh-hay-evacuaciones-masivas-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//espectaculos/musica/el-nuevo-album-de-david-gilmour-entre-la-finitud-el-trabajo-en-familia-y-el-infaltable-toque-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/aerolineas-apunto-a-los-gremios-por-el-paro-revelo-cuanto-ganan-los-pilotos-e-insistio-con-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//salud/por-que-conectamos-mas-con-las-criticas-que-con-los-elogios-y-repetimos-conductas-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//sabado/en-francia-100-puntos-para-un-malbec-argentino-en-el-mercado-de-vinos-de-lujo-mas-top-del-mundo-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//salud/bailar-tango-hace-bien-los-beneficios-desconocidos-que-genera-en-la-salud-emocional-de-quienes-se-nid04092024/</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/javier-milei-ya-dio-casi-seis-vueltas-al-mundo-desde-que-es-presidente-y-gasto-us24-millones-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//salud/nutricion/oro-blanco-el-probiotico-natural-perfecto-para-aumentar-las-defensas-y-mejorar-el-estado-de-animo-nid03092024/</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/dolar/dolar-hoy-dolar-blue-hoy-a-cuanto-cotiza-este-viernes-6-de-septiembre-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//salud/vida_sana/termas-el-mapa-argentino-de-aguas-curativas-con-multiples-beneficios-nid01092024/</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//propiedades/5-joyas-para-vivir-en-la-ciudad-de-buenos-aires-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//autos/cuanto-cuesta-la-ford-ranger-en-septiembre-2024-luego-de-la-baja-del-impuesto-pais-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/turf/triple-corona-del-turf-fue-alumno-de-la-jocketa-argentina-mas-ilustre-y-corre-a-colifato-novo-el-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//autos/cuanto-cuestan-las-pick-ups-en-septiembre-luego-de-la-baja-de-precios-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/segun-el-vice-del-bcra-enamorados-estamos-de-nuestras-mujeres-del-cepo-nos-hubiera-gustado-salir-nid05092024/</t>
+          <t>https://www.lanacion.com.ar//autos/las-motos-se-suman-a-la-baja-de-precios-cuales-son-los-modelos-que-retrocedieron-en-septiembre-nid04092024/</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/negocios/los-argentinos-que-lograron-establecerse-en-la-economia-mas-grande-de-la-union-europea-nid02092024/</t>
+          <t>https://www.lanacion.com.ar//autos/cuanto-cuesta-el-toyota-corolla-cross-en-septiembre-2024-luego-de-la-baja-del-impuesto-pais-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/negocios/los-planes-de-la-nueva-presidente-de-dow-en-la-argentina-nid03092024/</t>
+          <t>https://www.lanacion.com.ar//propiedades/construccion-y-diseno/historias-es-argentino-se-anticipo-a-un-megaproyecto-petrolero-y-desarrollo-la-ciudad-que-potenciara-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/negocios/anuncio-de-local-mercado-libre-invertira-us75-millones-en-un-centro-de-almacenamiento-nid04092024/</t>
+          <t>https://www.lanacion.com.ar//propiedades/casas-y-departamentos/la-ciudad-de-nueva-york-que-paga-us9000-por-mudarse-cuales-son-los-requisitos-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/radio/juan-alberto-mateyko-se-alejo-de-su-programa-de-radio-por-una-semana-y-debe-hacer-reposo-los-motivos-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//propiedades/casas-y-departamentos/primera-casa-se-mudan-a-un-convento-de-monjas-que-se-transformo-en-departamentos-para-jovenes-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/personajes/en-fotos-de-los-vestidos-reveladores-de-nicole-kidman-y-juliette-lewis-al-desembarco-gotico-en-el-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//propiedades/casas-y-departamentos/el-barrio-verde-que-vive-un-boom-de-construccion-y-tiene-hasta-dos-proyectos-en-una-misma-cuadra-nid02092024/</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/musica/el-nuevo-album-de-david-gilmour-entre-la-finitud-el-trabajo-en-familia-y-el-infaltable-toque-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//economia/campo/logro-del-conicet-revelaron-detalles-de-un-proceso-que-podria-ser-clave-para-el-futuro-de-los-nid04092024/</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//salud/bailar-tango-hace-bien-los-beneficios-desconocidos-que-genera-en-la-salud-emocional-de-quienes-se-nid04092024/</t>
+          <t>https://www.lanacion.com.ar//economia/campo/brutal-atentado-criminal-la-rural-exigio-a-la-justicia-el-mas-inmediato-esclarecimiento-del-ataque-a-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//salud/nutricion/oro-blanco-el-probiotico-natural-perfecto-para-aumentar-las-defensas-y-mejorar-el-estado-de-animo-nid03092024/</t>
+          <t>https://www.lanacion.com.ar//economia/campo/131-islas-malvinas-productores-firmaron-un-duro-documento-contra-europa-a-la-que-acusan-de-degradar-nid05092024/</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//salud/vida_sana/termas-el-mapa-argentino-de-aguas-curativas-con-multiples-beneficios-nid01092024/</t>
+          <t>https://www.lanacion.com.ar//economia/campo/paritaria-aceitera-cuanto-pasaran-a-ganar-los-trabajadores-de-uno-de-los-sectores-con-mejores-nid05092024/</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//salud/descanso/por-que-tener-hambre-o-bostezar-pueden-anunciar-una-migrana-nid04092024/</t>
+          <t>https://www.lanacion.com.ar//lifestyle/tras-volver-a-argentina-tomo-una-decision-y-tuvo-una-idea-para-el-pais-lo-vivido-en-alemania-nos-nid02092024/</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//autos/cuanto-cuesta-el-toyota-corolla-cross-en-septiembre-2024-luego-de-la-baja-del-impuesto-pais-nid06092024/</t>
+          <t>https://www.lanacion.com.ar//lifestyle/se-enamoraron-en-italia-en-argentina-un-suceso-oscuro-los-alejo-y-30-anos-despues-llegaron-las-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//autos/stellantis-invertira-us385-millones-en-cordoba-para-fabricar-nuevos-modelos-y-un-motor-nid05092024/</t>
+          <t>https://www.lanacion.com.ar//sabado/picada-cheta-y-budin-de-banana-split-el-comedor-gourmet-de-villa-fiorito-que-sorprendio-en-arteba-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//autos/renault-sorprendio-con-rebajas-de-hasta-un-23-en-algunos-modelos-nid04092024/</t>
+          <t>https://www.lanacion.com.ar//revista-living/conoce-la-casa-de-la-influencer-coty-crotto-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//autos/las-motos-se-suman-a-la-baja-de-precios-cuales-son-los-modelos-que-retrocedieron-en-septiembre-nid04092024/</t>
+          <t>https://www.lanacion.com.ar//revista-lugares/el-ultimo-guardian-de-la-paz-la-emotiva-lucha-por-salvar-una-de-las-pulperias-mas-antiguas-de-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//propiedades/casas-y-departamentos/el-barrio-verde-que-vive-un-boom-de-construccion-y-tiene-hasta-dos-proyectos-en-una-misma-cuadra-nid02092024/</t>
+          <t>https://www.lanacion.com.ar//feriados/2024/dia-del-maestro-el-11-de-septiembre-es-feriado-nid05092024/</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//propiedades/casas-y-departamentos/los-6-barrios-portenos-con-oportunidades-porque-los-departamentos-bajaron-de-precio-nid04092024/</t>
+          <t>https://www.lanacion.com.ar//espectaculos/musica/el-ultimo-recital-de-los-piojos-la-lista-de-canciones-nid05092024/</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//propiedades/inversiones/blanqueo-si-la-decision-es-comprar-una-propiedad-que-hay-que-analizar-para-no-perder-plata-nid04092024/</t>
+          <t>https://www.lanacion.com.ar//espectaculos/cuando-es-la-ceremonia-de-los-martin-fierro-2024-dia-y-horario-nid05092024/</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
-        <is>
-          <t>https://www.lanacion.com.ar//propiedades/casas-y-departamentos/cristiano-ronaldo-como-es-el-palacio-moderno-que-compro-por-25-millones-de-euros-en-dubai-nid05092024/</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>https://www.lanacion.com.ar//economia/campo/brutal-atentado-criminal-la-rural-exigio-a-la-justicia-el-mas-inmediato-esclarecimiento-del-ataque-a-nid06092024/</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>https://www.lanacion.com.ar//economia/campo/131-islas-malvinas-productores-firmaron-un-duro-documento-contra-europa-a-la-que-acusan-de-degradar-nid05092024/</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>https://www.lanacion.com.ar//economia/campo/paritaria-aceitera-cuanto-pasaran-a-ganar-los-trabajadores-de-uno-de-los-sectores-con-mejores-nid05092024/</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>https://www.lanacion.com.ar//economia/campo/resistente-a-dos-poderosos-virus-se-viene-un-nuevo-desarrollo-argentino-para-la-papa-nid04092024/</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>https://www.lanacion.com.ar//lifestyle/presencio-como-la-ataban-a-un-arbol-y-la-abandonaban-pero-cuando-se-acerco-entendio-la-triste-nid01092024/</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>https://www.lanacion.com.ar//lifestyle/agresion-a-su-madre-relaciones-fallidas-y-arrestos-la-turbulenta-vida-del-hijo-mayor-de-nicolas-cage-nid05092024/</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>https://www.lanacion.com.ar//lifestyle/en-fotos-todos-los-invitados-al-cocktail-de-javier-saiach-por-el-cierre-de-su-tienda-en-recoleta-nid05092024/</t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>https://www.lanacion.com.ar//revista-lugares/el-ultimo-guardian-de-la-paz-la-emotiva-lucha-por-salvar-una-de-las-pulperias-mas-antiguas-de-nid06092024/</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>https://www.lanacion.com.ar//revista-jardin/por-que-las-colocasias-mueren-en-invierno-y-como-evitarlo-nid04092024/</t>
-        </is>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>https://www.lanacion.com.ar//feriados/2024/dia-del-maestro-el-11-de-septiembre-es-feriado-nid05092024/</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>https://www.lanacion.com.ar//espectaculos/musica/el-ultimo-recital-de-los-piojos-la-lista-de-canciones-nid05092024/</t>
-        </is>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>https://www.lanacion.com.ar//espectaculos/cuando-es-la-ceremonia-de-los-martin-fierro-2024-dia-y-horario-nid05092024/</t>
-        </is>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="inlineStr">
         <is>
           <t>https://www.lanacion.com.ar//clima/el-clima-en-el-amba-como-estara-el-tiempo-durante-el-fin-de-semana-del-viernes-6-de-septiembre-nid05092024/</t>
         </is>

</xml_diff>